<commit_message>
Integrated Piecewise linear regression into PCR code
</commit_message>
<xml_diff>
--- a/BillOfMaterials.xlsx
+++ b/BillOfMaterials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamno\PCR\FortLewis_PCR-TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBCCFC8-3200-4B87-BC8A-41B3F5BB135C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16777141-9699-4012-88B6-7133DFF4946F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4FD58BD-C2F8-42AE-A30D-9012D714C2B3}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +495,7 @@
         <v>9.99</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -507,6 +507,9 @@
       </c>
       <c r="B4">
         <v>7.5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>

</xml_diff>